<commit_message>
I think so (FB_Side code might be djank but works
</commit_message>
<xml_diff>
--- a/ExaminerTools/Docs and Forms/Attendance&Timekeeping_RND2.xlsx
+++ b/ExaminerTools/Docs and Forms/Attendance&Timekeeping_RND2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="50">
   <si>
     <t xml:space="preserve">Restoring Natural Touch to Active Prosthesis Users: </t>
   </si>
@@ -162,22 +162,22 @@
     <t>TBD:</t>
   </si>
   <si>
-    <t>Arturs</t>
-  </si>
-  <si>
     <t>George</t>
   </si>
   <si>
     <t>Finn</t>
   </si>
   <si>
-    <t>Carol</t>
-  </si>
-  <si>
     <t>Frasier</t>
   </si>
   <si>
     <t>Chris</t>
+  </si>
+  <si>
+    <t>Carol Lo - 028</t>
+  </si>
+  <si>
+    <t>Patrick Brinson - 029</t>
   </si>
 </sst>
 </file>
@@ -281,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -925,6 +925,36 @@
       <left style="thin">
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </left>
+      <right style="medium">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="dashed">
         <color indexed="64"/>
@@ -935,6 +965,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </left>
@@ -944,8 +987,75 @@
       <top style="thin">
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -956,8 +1066,17 @@
       <right style="medium">
         <color theme="2" tint="-0.499984740745262"/>
       </right>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="dashed">
         <color indexed="64"/>
@@ -965,42 +1084,144 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="dashed">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="dashed">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="dashed">
         <color indexed="64"/>
       </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </bottom>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1013,56 +1234,13 @@
       <top style="dashed">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </left>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color theme="2" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -1074,14 +1252,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1089,18 +1264,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1163,31 +1326,175 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1196,154 +1503,76 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1626,343 +1855,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="4" customWidth="1"/>
-    <col min="2" max="7" width="25.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" style="4" customWidth="1"/>
-    <col min="11" max="29" width="10.28515625" style="4" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.28515625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="25.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" style="3" customWidth="1"/>
+    <col min="11" max="29" width="10.28515625" style="3" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="1"/>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="S1" s="3"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="4" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="4" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="82"/>
+      <c r="D8" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="29" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="4" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="86"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="71"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="85"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="107"/>
     </row>
     <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="106"/>
     </row>
     <row r="12" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="29" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="66"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="56"/>
     </row>
     <row r="14" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30" t="s">
+      <c r="C14" s="105"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="26" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="71"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="61"/>
     </row>
     <row r="16" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="30" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="48"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="81"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="70"/>
     </row>
     <row r="18" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="29" t="s">
+      <c r="D18" s="53"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="82"/>
+      <c r="G18" s="107"/>
     </row>
     <row r="19" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="83"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="89"/>
     </row>
     <row r="20" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="4" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="4" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="A1:G1"/>
@@ -1972,6 +2195,8 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1983,319 +2208,330 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="4" customWidth="1"/>
-    <col min="2" max="7" width="25.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" style="4" customWidth="1"/>
-    <col min="11" max="29" width="10.28515625" style="4" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.28515625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="25.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" style="3" customWidth="1"/>
+    <col min="11" max="29" width="10.28515625" style="3" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="1"/>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="S1" s="3"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="4" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="4" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="29" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="4" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="87"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="72"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="56"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="88"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="84"/>
     </row>
     <row r="12" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="29" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="66"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="56"/>
     </row>
     <row r="14" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="29" t="s">
+      <c r="C14" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="24" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="29" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="48"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="76"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="66"/>
     </row>
     <row r="18" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="89"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="29" t="s">
+      <c r="D18" s="73"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="77"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="51"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D14:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2307,312 +2543,322 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="4" customWidth="1"/>
-    <col min="2" max="7" width="25.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" style="4" customWidth="1"/>
-    <col min="11" max="29" width="10.28515625" style="4" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.28515625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="25.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" style="3" customWidth="1"/>
+    <col min="11" max="29" width="10.28515625" style="3" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="1"/>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="S1" s="3"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="4" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="4" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="29" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="4" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="86"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="71"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="85"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="84"/>
     </row>
     <row r="12" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="29" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="64"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="54" t="s">
+      <c r="C14" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="24" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="52"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="42"/>
     </row>
     <row r="16" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="29" t="s">
+      <c r="C16" s="93"/>
+      <c r="D16" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
     </row>
     <row r="17" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="23"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="90"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="29" t="s">
+      <c r="D18" s="74"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="71"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="61"/>
     </row>
     <row r="20" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2630,312 +2876,322 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="4" customWidth="1"/>
-    <col min="2" max="7" width="25.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" style="4" customWidth="1"/>
-    <col min="11" max="29" width="10.28515625" style="4" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.28515625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="25.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" style="3" customWidth="1"/>
+    <col min="11" max="29" width="10.28515625" style="3" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="1"/>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="S1" s="3"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="4" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="4" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="30" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="24"/>
-      <c r="J8" s="4" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="31"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="76"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="84"/>
     </row>
     <row r="12" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="30" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="75" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="31"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="76"/>
     </row>
     <row r="14" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="29" t="s">
+      <c r="C14" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="75" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="31"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="76"/>
     </row>
     <row r="16" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="29" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="23"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="23"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="89"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="30" t="s">
+      <c r="D18" s="73"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="71"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="61"/>
     </row>
     <row r="20" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="48"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2957,300 +3213,311 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="4" customWidth="1"/>
-    <col min="2" max="7" width="25.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" style="4" customWidth="1"/>
-    <col min="11" max="29" width="10.28515625" style="4" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.28515625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="25.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" style="3" customWidth="1"/>
+    <col min="11" max="29" width="10.28515625" style="3" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="1"/>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="S1" s="3"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="4" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="4" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="4" t="s">
+      <c r="D8" s="49"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="29" t="s">
+      <c r="C10" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="75" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="76"/>
     </row>
     <row r="12" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
+      <c r="C14" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="23"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="30" t="s">
+      <c r="C18" s="63"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="75" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="31"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="76"/>
     </row>
     <row r="20" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="51"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="2:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>